<commit_message>
chore(input): add sample sheet parse, empty checks
</commit_message>
<xml_diff>
--- a/templates/production/SampleSheet.xlsx
+++ b/templates/production/SampleSheet.xlsx
@@ -215,7 +215,7 @@
     <t>String, no whitespaces, unique for this sample sheet</t>
   </si>
   <si>
-    <t>Numeric, YYYYMMDD</t>
+    <t>Integer, YYYYMMDD</t>
   </si>
   <si>
     <t>String, no whitespaces, unique across all runs</t>
@@ -227,13 +227,20 @@
     <t>String, no tab delimiter</t>
   </si>
   <si>
-    <t>Numeric (picogram)</t>
+    <t>Float (picogram)</t>
   </si>
   <si>
     <t>Recommended format</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Unique across all data; DNA/RNA/NTC tags used. Modular sample identifier that works best with Cerebro UI: (1) biological sample identifier, i.e. the identifier that can link this library to the biological sample (2) Double underscore separator (3) One of the following nucleic acid tags of the library: DNA or RNA (4) Double underscore separator (5) Additional libary tag, usually NTC if negative template control (6)  Double underscore separator (7) any additional tags that should make up the unique tag combination for this sample (8) </t>
     </r>
     <r>
@@ -287,6 +294,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>DW-63-76__DNA__NTC_S32</t>
     </r>
     <r>
@@ -412,10 +426,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -442,41 +456,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -488,23 +472,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -526,9 +511,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -542,14 +548,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -557,22 +586,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -587,187 +601,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -790,17 +804,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -816,6 +824,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -846,21 +869,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -870,11 +878,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -883,142 +897,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2409,7 +2423,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.225" defaultRowHeight="14.25" outlineLevelRow="5"/>

</xml_diff>

<commit_message>
chore(input): format validation check msg
</commit_message>
<xml_diff>
--- a/templates/production/SampleSheet.xlsx
+++ b/templates/production/SampleSheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="82">
   <si>
     <t>sample_id</t>
   </si>
@@ -276,9 +276,6 @@
   </si>
   <si>
     <t>MGP-20231010007</t>
-  </si>
-  <si>
-    <t>TRUE, FALSE</t>
   </si>
   <si>
     <t>Library preparation was done on 80ul input instead of 100ul input due to lack of primary sample</t>
@@ -2422,8 +2419,8 @@
   <sheetPr/>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.225" defaultRowHeight="14.25" outlineLevelRow="5"/>
@@ -2559,17 +2556,17 @@
       <c r="D5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="I5" s="1">
         <v>25</v>
@@ -2577,10 +2574,10 @@
     </row>
     <row r="6" ht="256.5" spans="1:9">
       <c r="A6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>73</v>

</xml_diff>